<commit_message>
Adding the new data to the charts.
</commit_message>
<xml_diff>
--- a/data/Android Battery Charts.xlsx
+++ b/data/Android Battery Charts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Estimated Time Remaining 1" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,15 @@
     <sheet name="Battery Level 2" sheetId="5" r:id="rId4"/>
     <sheet name="Estimated Time Remaining 3" sheetId="7" r:id="rId5"/>
     <sheet name="Battery Level 3" sheetId="8" r:id="rId6"/>
+    <sheet name="Estimated Time Remaining 4" sheetId="9" r:id="rId7"/>
+    <sheet name="Battery Level 4" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="7">
   <si>
     <t>short</t>
   </si>
@@ -75,11 +77,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -328,11 +331,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="134660672"/>
-        <c:axId val="134661248"/>
+        <c:axId val="112741184"/>
+        <c:axId val="112741760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="134660672"/>
+        <c:axId val="112741184"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -342,12 +345,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134661248"/>
+        <c:crossAx val="112741760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="134661248"/>
+        <c:axId val="112741760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -358,7 +361,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134660672"/>
+        <c:crossAx val="112741184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -368,6 +371,1306 @@
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Estimated Time Remaining 4'!$F$2:$F$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.77</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Estimated Time Remaining 4'!$J$2:$J$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>7.9355347222222052</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40.365737499999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.098603015873046</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.993175888888889</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.47341876068376</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.432779555555548</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27.01765565972223</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.6666444444444473</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27.543411695906439</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.4167736111111084</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="124772928"/>
+        <c:axId val="124773504"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="124772928"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="124773504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="124773504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="124772928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Estimated Time Remaining</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Estimated Time Remaining 4'!$C$2:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.66660666669486091</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3331947222468443</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.999937777814921</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6664669444435276</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5085644444916397</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.1752194444416091</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.8418869444867596</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.5085569444927387</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.0085544444737025</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Estimated Time Remaining 4'!$J$2:$J$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>7.9355347222222052</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40.365737499999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.098603015873046</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.993175888888889</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.47341876068376</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.432779555555548</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27.01765565972223</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.6666444444444473</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27.543411695906439</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.4167736111111084</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="124775808"/>
+        <c:axId val="124776384"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="124775808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Running (hours)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="124776384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="124776384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Left till dead (hours)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="124775808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Battery Level</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.9900304081468864E-2"/>
+                  <c:y val="-0.66127008310443003"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.7506948098078904E-2"/>
+                  <c:y val="-0.47697411729637795"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Battery Level 4'!$B$2:$B$259</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="258"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.329333335859701E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16671138891251758</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25016333331586793</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.33329361112555489</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.44962527777533978</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.53296444442821667</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.61613388889236376</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.69961750000948086</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.78322666668100283</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.86628277780255303</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.94947138888528571</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.0330033333157189</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1165611111209728</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.1995508333202451</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.2828236111090519</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.3663341666688211</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.4494697222253308</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.532803611131385</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.6161355555523187</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.6996100000105798</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.7828033333062194</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.8662886111414991</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.9496547222370282</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.032946944469586</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.1161361110862345</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.1996077777585015</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.2829413888975978</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.3661980555625632</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.4498925000079907</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.5328033333062194</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.616279722249601</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.6996116666705348</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.7832247221958824</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.8661369444453157</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.9494674999732524</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.0329411111306399</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.1165513888699934</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.1994716666522436</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.2829463888774626</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.3666722222114913</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3.4494800000102259</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.532940833363682</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.6162736110854894</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.6994702777592465</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3.7830019444227219</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.8665524999960326</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3.9582250000094064</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.0415633333614096</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.1248872222495265</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.2082205555634573</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4.2916327777784318</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4.3751655555679463</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4.4582224999903701</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4.5415677778073587</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4.6251630555489101</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.7082208333304152</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4.7918511111056432</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4.8748872222495265</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4.9582208333304152</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>5.0415558333625086</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>5.1248972222092561</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>5.208222777757328</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>5.2915552777703851</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>5.3748988888692111</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>5.4582205555634573</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>5.5416049999766983</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>5.6251719444408081</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>5.7082816666807048</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>5.791557222197298</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>5.8748902778024785</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>5.9582291666883975</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>6.0416813889169134</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>6.1252144444733858</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>6.2083058333373629</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>6.2918375000008382</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>6.375173888867721</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>6.4582672222168185</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>6.5415602778084576</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>6.6249563888995908</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>6.7082238888833672</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>6.7916002777637914</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>6.874889999977313</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>6.9582230555824935</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>7.0415577777894214</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Battery Level 4'!$C$2:$C$259</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="258"/>
+                <c:pt idx="0">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.77</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="124778112"/>
+        <c:axId val="124778688"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="124778112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="7"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Running (hours)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="124778688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="124778688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.75000000000000011"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Battery Level</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="124778112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.0782734830852821E-2"/>
+          <c:y val="0.13185289107421672"/>
+          <c:w val="0.87921729489363087"/>
+          <c:h val="0.72319861787446382"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Estimated Time Remaining</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Estimated Time Remaining 4'!$C$2:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.66660666669486091</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3331947222468443</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.999937777814921</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6664669444435276</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5085644444916397</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.1752194444416091</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.8418869444867596</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.5085569444927387</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.0085544444737025</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Estimated Time Remaining 4'!$J$2:$J$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>7.9355347222222052</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40.365737499999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.098603015873046</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.993175888888889</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.47341876068376</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.432779555555548</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27.01765565972223</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.6666444444444473</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27.543411695906439</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.4167736111111084</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="127699200"/>
+        <c:axId val="127699776"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="127699200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Running (hours)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="127699776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="127699776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Left till dead (hours)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="127699200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -621,11 +1924,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="134662976"/>
-        <c:axId val="134663552"/>
+        <c:axId val="112743488"/>
+        <c:axId val="112744064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="134662976"/>
+        <c:axId val="112743488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -659,12 +1962,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134663552"/>
+        <c:crossAx val="112744064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="134663552"/>
+        <c:axId val="112744064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -699,7 +2002,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134662976"/>
+        <c:crossAx val="112743488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2325,11 +3628,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="134665280"/>
-        <c:axId val="134665856"/>
+        <c:axId val="112745792"/>
+        <c:axId val="115097600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="134665280"/>
+        <c:axId val="112745792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2363,12 +3666,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134665856"/>
+        <c:crossAx val="115097600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="134665856"/>
+        <c:axId val="115097600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2398,7 +3701,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134665280"/>
+        <c:crossAx val="112745792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2499,11 +3802,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="134667584"/>
-        <c:axId val="142123008"/>
+        <c:axId val="115099328"/>
+        <c:axId val="115099904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="134667584"/>
+        <c:axId val="115099328"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2513,12 +3816,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142123008"/>
+        <c:crossAx val="115099904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="142123008"/>
+        <c:axId val="115099904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2529,14 +3832,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134667584"/>
+        <c:crossAx val="115099328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2635,11 +3937,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="142124736"/>
-        <c:axId val="142125312"/>
+        <c:axId val="115101632"/>
+        <c:axId val="115102208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="142124736"/>
+        <c:axId val="115101632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2649,12 +3951,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142125312"/>
+        <c:crossAx val="115102208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="142125312"/>
+        <c:axId val="115102208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2665,14 +3967,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142124736"/>
+        <c:crossAx val="115101632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4346,11 +5647,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="142127040"/>
-        <c:axId val="142127616"/>
+        <c:axId val="115103936"/>
+        <c:axId val="115104512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="142127040"/>
+        <c:axId val="115103936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4360,12 +5661,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142127616"/>
+        <c:crossAx val="115104512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="142127616"/>
+        <c:axId val="115104512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4376,14 +5677,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142127040"/>
+        <c:crossAx val="115103936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4458,11 +5758,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="144510336"/>
-        <c:axId val="144510912"/>
+        <c:axId val="116499008"/>
+        <c:axId val="116499584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="144510336"/>
+        <c:axId val="116499008"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4472,12 +5772,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144510912"/>
+        <c:crossAx val="116499584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="144510912"/>
+        <c:axId val="116499584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4488,14 +5788,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144510336"/>
+        <c:crossAx val="116499008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4570,11 +5869,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="144513216"/>
-        <c:axId val="144513792"/>
+        <c:axId val="116501312"/>
+        <c:axId val="116501888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="144513216"/>
+        <c:axId val="116501312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4584,12 +5883,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144513792"/>
+        <c:crossAx val="116501888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="144513792"/>
+        <c:axId val="116501888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4600,14 +5899,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144513216"/>
+        <c:crossAx val="116501312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4714,11 +6012,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="144508032"/>
-        <c:axId val="144508608"/>
+        <c:axId val="116503616"/>
+        <c:axId val="116504192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="144508032"/>
+        <c:axId val="116503616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4728,12 +6026,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144508608"/>
+        <c:crossAx val="116504192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="144508608"/>
+        <c:axId val="116504192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4744,14 +6042,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144508032"/>
+        <c:crossAx val="116503616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5078,6 +6375,144 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>42861</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>523874</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>14288</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5367,7 +6802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView topLeftCell="I26" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -6394,7 +7829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
@@ -14662,4 +16097,2401 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AC32"/>
+  <sheetViews>
+    <sheetView topLeftCell="G7" workbookViewId="0">
+      <selection activeCell="Z23" sqref="Z23:AD32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C1">
+        <f>B2/(1000*3600)</f>
+        <v>376431.57340333331</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1355153664252</v>
+      </c>
+      <c r="C2" s="2">
+        <f>B2/(1000*3600)-$C$1</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3.3254077781287999E-8</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1.0756123192030199E-8</v>
+      </c>
+      <c r="F2">
+        <v>0.95</v>
+      </c>
+      <c r="H2">
+        <f>IF(D2=0,F2/E2,F2/D2)</f>
+        <v>28567924.99999994</v>
+      </c>
+      <c r="I2">
+        <f>H2/(1000*60)</f>
+        <v>476.13208333333233</v>
+      </c>
+      <c r="J2">
+        <f>I2/60</f>
+        <v>7.9355347222222052</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1355156064036</v>
+      </c>
+      <c r="C3" s="2">
+        <f t="shared" ref="C3:C31" si="0">B3/(1000*3600)-$C$1</f>
+        <v>0.66660666669486091</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>6.5374474797813099E-9</v>
+      </c>
+      <c r="F3">
+        <v>0.95</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H31" si="1">IF(D3=0,F3/E3,F3/D3)</f>
+        <v>145316654.99999997</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I31" si="2">H3/(1000*60)</f>
+        <v>2421.9442499999996</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J31" si="3">I3/60</f>
+        <v>40.365737499999994</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1355158463753</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" si="0"/>
+        <v>1.3331947222468443</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>8.2175895626281795E-9</v>
+      </c>
+      <c r="F4">
+        <v>0.92</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>111954970.85714297</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>1865.9161809523828</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="3"/>
+        <v>31.098603015873046</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1355160864028</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" si="0"/>
+        <v>1.999937777814921</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>9.1586934134706803E-9</v>
+      </c>
+      <c r="F5">
+        <v>0.89</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>97175433.199999988</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>1619.5905533333332</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="3"/>
+        <v>26.993175888888889</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1355163263533</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" si="0"/>
+        <v>2.6664669444435276</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>9.7611572467619802E-9</v>
+      </c>
+      <c r="F6">
+        <v>0.86</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>88104307.538461536</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>1468.4051256410255</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>24.47341876068376</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1355166295084</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" si="0"/>
+        <v>3.5085644444916397</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>9.1745116896734898E-9</v>
+      </c>
+      <c r="F7">
+        <v>0.84</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>91558006.399999976</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>1525.9667733333329</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>25.432779555555548</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1355168695042</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>4.1752194444416091</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>8.5335144714005095E-9</v>
+      </c>
+      <c r="F8">
+        <v>0.83</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>97263560.37500003</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>1621.0593395833339</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>27.01765565972223</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1355171095045</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>4.8418869444867596</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3.33334444448148E-8</v>
+      </c>
+      <c r="E9" s="1">
+        <v>8.9836193158217407E-9</v>
+      </c>
+      <c r="F9">
+        <v>0.8</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>23999920.000000011</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>399.99866666666685</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>6.6666444444444473</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1355173495057</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>5.5085569444927387</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>8.0680717652435693E-9</v>
+      </c>
+      <c r="F10">
+        <v>0.8</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>99156282.105263174</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>1652.6047017543863</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>27.543411695906439</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1355175295048</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>6.0085544444737025</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3.3332777787036899E-8</v>
+      </c>
+      <c r="E11" s="1">
+        <v>8.6786351883626696E-9</v>
+      </c>
+      <c r="F11">
+        <v>0.77</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>23100384.999999989</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>385.0064166666665</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>6.4167736111111084</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="E23" s="1"/>
+      <c r="AB23" s="1"/>
+      <c r="AC23" s="1"/>
+    </row>
+    <row r="24" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="E24" s="1"/>
+      <c r="AC24" s="1"/>
+    </row>
+    <row r="25" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="AC25" s="1"/>
+    </row>
+    <row r="26" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="E26" s="1"/>
+      <c r="AC26" s="1"/>
+    </row>
+    <row r="27" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="E27" s="1"/>
+      <c r="AC27" s="1"/>
+    </row>
+    <row r="28" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="E28" s="1"/>
+      <c r="AC28" s="1"/>
+    </row>
+    <row r="29" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="E29" s="1"/>
+      <c r="AC29" s="1"/>
+    </row>
+    <row r="30" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="E30" s="1"/>
+      <c r="AB30" s="1"/>
+      <c r="AC30" s="1"/>
+    </row>
+    <row r="31" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="E31" s="1"/>
+      <c r="AC31" s="1"/>
+    </row>
+    <row r="32" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AB32" s="1"/>
+      <c r="AC32" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D259"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <f>A2/(1000*3600)</f>
+        <v>376430.5404</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1355149945440</v>
+      </c>
+      <c r="B2" s="2">
+        <f>A2/(1000*3600)-$D$1</f>
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>1355150245296</v>
+      </c>
+      <c r="B3" s="2">
+        <f t="shared" ref="B3:B66" si="0">A3/(1000*3600)-$D$1</f>
+        <v>8.329333335859701E-2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>1355150545601</v>
+      </c>
+      <c r="B4" s="2">
+        <f t="shared" si="0"/>
+        <v>0.16671138891251758</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>1355150846028</v>
+      </c>
+      <c r="B5" s="2">
+        <f t="shared" si="0"/>
+        <v>0.25016333331586793</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>1355151145297</v>
+      </c>
+      <c r="B6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.33329361112555489</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>1355151564091</v>
+      </c>
+      <c r="B7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.44962527777533978</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>1355151864112</v>
+      </c>
+      <c r="B8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.53296444442821667</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>1355152163522</v>
+      </c>
+      <c r="B9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.61613388889236376</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>1355152464063</v>
+      </c>
+      <c r="B10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.69961750000948086</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>1355152765056</v>
+      </c>
+      <c r="B11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.78322666668100283</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>1355153064058</v>
+      </c>
+      <c r="B12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.86628277780255303</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>1355153363537</v>
+      </c>
+      <c r="B13" s="2">
+        <f t="shared" si="0"/>
+        <v>0.94947138888528571</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>1355153664252</v>
+      </c>
+      <c r="B14" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0330033333157189</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>1355153965060</v>
+      </c>
+      <c r="B15" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1165611111209728</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>1355154263823</v>
+      </c>
+      <c r="B16" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1995508333202451</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>1355154563605</v>
+      </c>
+      <c r="B17" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2828236111090519</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>1355154864243</v>
+      </c>
+      <c r="B18" s="2">
+        <f t="shared" si="0"/>
+        <v>1.3663341666688211</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>1355155163531</v>
+      </c>
+      <c r="B19" s="2">
+        <f t="shared" si="0"/>
+        <v>1.4494697222253308</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>1355155463533</v>
+      </c>
+      <c r="B20" s="2">
+        <f t="shared" si="0"/>
+        <v>1.532803611131385</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>1355155763528</v>
+      </c>
+      <c r="B21" s="2">
+        <f t="shared" si="0"/>
+        <v>1.6161355555523187</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>1355156064036</v>
+      </c>
+      <c r="B22" s="2">
+        <f t="shared" si="0"/>
+        <v>1.6996100000105798</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>1355156363532</v>
+      </c>
+      <c r="B23" s="2">
+        <f t="shared" si="0"/>
+        <v>1.7828033333062194</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>1355156664079</v>
+      </c>
+      <c r="B24" s="2">
+        <f t="shared" si="0"/>
+        <v>1.8662886111414991</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>1355156964197</v>
+      </c>
+      <c r="B25" s="2">
+        <f t="shared" si="0"/>
+        <v>1.9496547222370282</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>1355157264049</v>
+      </c>
+      <c r="B26" s="2">
+        <f t="shared" si="0"/>
+        <v>2.032946944469586</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>1355157563530</v>
+      </c>
+      <c r="B27" s="2">
+        <f t="shared" si="0"/>
+        <v>2.1161361110862345</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>1355157864028</v>
+      </c>
+      <c r="B28" s="2">
+        <f t="shared" si="0"/>
+        <v>2.1996077777585015</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>1355158164029</v>
+      </c>
+      <c r="B29" s="2">
+        <f t="shared" si="0"/>
+        <v>2.2829413888975978</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>1355158463753</v>
+      </c>
+      <c r="B30" s="2">
+        <f t="shared" si="0"/>
+        <v>2.3661980555625632</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>1355158765053</v>
+      </c>
+      <c r="B31" s="2">
+        <f t="shared" si="0"/>
+        <v>2.4498925000079907</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>1355159063532</v>
+      </c>
+      <c r="B32" s="2">
+        <f t="shared" si="0"/>
+        <v>2.5328033333062194</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>1355159364047</v>
+      </c>
+      <c r="B33" s="2">
+        <f t="shared" si="0"/>
+        <v>2.616279722249601</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>1355159664042</v>
+      </c>
+      <c r="B34" s="2">
+        <f t="shared" si="0"/>
+        <v>2.6996116666705348</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>1355159965049</v>
+      </c>
+      <c r="B35" s="2">
+        <f t="shared" si="0"/>
+        <v>2.7832247221958824</v>
+      </c>
+      <c r="C35" s="3">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>1355160263533</v>
+      </c>
+      <c r="B36" s="2">
+        <f t="shared" si="0"/>
+        <v>2.8661369444453157</v>
+      </c>
+      <c r="C36" s="3">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>1355160563523</v>
+      </c>
+      <c r="B37" s="2">
+        <f t="shared" si="0"/>
+        <v>2.9494674999732524</v>
+      </c>
+      <c r="C37" s="3">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>1355160864028</v>
+      </c>
+      <c r="B38" s="2">
+        <f t="shared" si="0"/>
+        <v>3.0329411111306399</v>
+      </c>
+      <c r="C38" s="3">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>1355161165025</v>
+      </c>
+      <c r="B39" s="2">
+        <f t="shared" si="0"/>
+        <v>3.1165513888699934</v>
+      </c>
+      <c r="C39" s="3">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>1355161463538</v>
+      </c>
+      <c r="B40" s="2">
+        <f t="shared" si="0"/>
+        <v>3.1994716666522436</v>
+      </c>
+      <c r="C40" s="3">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>1355161764047</v>
+      </c>
+      <c r="B41" s="2">
+        <f t="shared" si="0"/>
+        <v>3.2829463888774626</v>
+      </c>
+      <c r="C41" s="3">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>1355162065460</v>
+      </c>
+      <c r="B42" s="2">
+        <f t="shared" si="0"/>
+        <v>3.3666722222114913</v>
+      </c>
+      <c r="C42" s="3">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>1355162363568</v>
+      </c>
+      <c r="B43" s="2">
+        <f t="shared" si="0"/>
+        <v>3.4494800000102259</v>
+      </c>
+      <c r="C43" s="3">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>1355162664027</v>
+      </c>
+      <c r="B44" s="2">
+        <f t="shared" si="0"/>
+        <v>3.532940833363682</v>
+      </c>
+      <c r="C44" s="3">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>1355162964025</v>
+      </c>
+      <c r="B45" s="2">
+        <f t="shared" si="0"/>
+        <v>3.6162736110854894</v>
+      </c>
+      <c r="C45" s="3">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>1355163263533</v>
+      </c>
+      <c r="B46" s="2">
+        <f t="shared" si="0"/>
+        <v>3.6994702777592465</v>
+      </c>
+      <c r="C46" s="3">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>1355163564247</v>
+      </c>
+      <c r="B47" s="2">
+        <f t="shared" si="0"/>
+        <v>3.7830019444227219</v>
+      </c>
+      <c r="C47" s="3">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>1355163865029</v>
+      </c>
+      <c r="B48" s="2">
+        <f t="shared" si="0"/>
+        <v>3.8665524999960326</v>
+      </c>
+      <c r="C48" s="3">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>1355164195050</v>
+      </c>
+      <c r="B49" s="2">
+        <f t="shared" si="0"/>
+        <v>3.9582250000094064</v>
+      </c>
+      <c r="C49" s="3">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>1355164495068</v>
+      </c>
+      <c r="B50" s="2">
+        <f t="shared" si="0"/>
+        <v>4.0415633333614096</v>
+      </c>
+      <c r="C50" s="3">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>1355164795034</v>
+      </c>
+      <c r="B51" s="2">
+        <f t="shared" si="0"/>
+        <v>4.1248872222495265</v>
+      </c>
+      <c r="C51" s="3">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>1355165095034</v>
+      </c>
+      <c r="B52" s="2">
+        <f t="shared" si="0"/>
+        <v>4.2082205555634573</v>
+      </c>
+      <c r="C52" s="3">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>1355165395318</v>
+      </c>
+      <c r="B53" s="2">
+        <f t="shared" si="0"/>
+        <v>4.2916327777784318</v>
+      </c>
+      <c r="C53" s="3">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>1355165696036</v>
+      </c>
+      <c r="B54" s="2">
+        <f t="shared" si="0"/>
+        <v>4.3751655555679463</v>
+      </c>
+      <c r="C54" s="3">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <v>1355165995041</v>
+      </c>
+      <c r="B55" s="2">
+        <f t="shared" si="0"/>
+        <v>4.4582224999903701</v>
+      </c>
+      <c r="C55" s="3">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
+        <v>1355166295084</v>
+      </c>
+      <c r="B56" s="2">
+        <f t="shared" si="0"/>
+        <v>4.5415677778073587</v>
+      </c>
+      <c r="C56" s="3">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
+        <v>1355166596027</v>
+      </c>
+      <c r="B57" s="2">
+        <f t="shared" si="0"/>
+        <v>4.6251630555489101</v>
+      </c>
+      <c r="C57" s="3">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
+        <v>1355166895035</v>
+      </c>
+      <c r="B58" s="2">
+        <f t="shared" si="0"/>
+        <v>4.7082208333304152</v>
+      </c>
+      <c r="C58" s="3">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
+        <v>1355167196104</v>
+      </c>
+      <c r="B59" s="2">
+        <f t="shared" si="0"/>
+        <v>4.7918511111056432</v>
+      </c>
+      <c r="C59" s="3">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
+        <v>1355167495034</v>
+      </c>
+      <c r="B60" s="2">
+        <f t="shared" si="0"/>
+        <v>4.8748872222495265</v>
+      </c>
+      <c r="C60" s="3">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="4">
+        <v>1355167795035</v>
+      </c>
+      <c r="B61" s="2">
+        <f t="shared" si="0"/>
+        <v>4.9582208333304152</v>
+      </c>
+      <c r="C61" s="3">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="4">
+        <v>1355168095041</v>
+      </c>
+      <c r="B62" s="2">
+        <f t="shared" si="0"/>
+        <v>5.0415558333625086</v>
+      </c>
+      <c r="C62" s="3">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="4">
+        <v>1355168395070</v>
+      </c>
+      <c r="B63" s="2">
+        <f t="shared" si="0"/>
+        <v>5.1248972222092561</v>
+      </c>
+      <c r="C63" s="3">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="4">
+        <v>1355168695042</v>
+      </c>
+      <c r="B64" s="2">
+        <f t="shared" si="0"/>
+        <v>5.208222777757328</v>
+      </c>
+      <c r="C64" s="3">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="4">
+        <v>1355168995039</v>
+      </c>
+      <c r="B65" s="2">
+        <f t="shared" si="0"/>
+        <v>5.2915552777703851</v>
+      </c>
+      <c r="C65" s="3">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="4">
+        <v>1355169295076</v>
+      </c>
+      <c r="B66" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3748988888692111</v>
+      </c>
+      <c r="C66" s="3">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="4">
+        <v>1355169595034</v>
+      </c>
+      <c r="B67" s="2">
+        <f t="shared" ref="B67:B130" si="1">A67/(1000*3600)-$D$1</f>
+        <v>5.4582205555634573</v>
+      </c>
+      <c r="C67" s="3">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="4">
+        <v>1355169895218</v>
+      </c>
+      <c r="B68" s="2">
+        <f t="shared" si="1"/>
+        <v>5.5416049999766983</v>
+      </c>
+      <c r="C68" s="3">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="4">
+        <v>1355170196059</v>
+      </c>
+      <c r="B69" s="2">
+        <f t="shared" si="1"/>
+        <v>5.6251719444408081</v>
+      </c>
+      <c r="C69" s="3">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="4">
+        <v>1355170495254</v>
+      </c>
+      <c r="B70" s="2">
+        <f t="shared" si="1"/>
+        <v>5.7082816666807048</v>
+      </c>
+      <c r="C70" s="3">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="4">
+        <v>1355170795046</v>
+      </c>
+      <c r="B71" s="2">
+        <f t="shared" si="1"/>
+        <v>5.791557222197298</v>
+      </c>
+      <c r="C71" s="3">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="4">
+        <v>1355171095045</v>
+      </c>
+      <c r="B72" s="2">
+        <f t="shared" si="1"/>
+        <v>5.8748902778024785</v>
+      </c>
+      <c r="C72" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="4">
+        <v>1355171395065</v>
+      </c>
+      <c r="B73" s="2">
+        <f t="shared" si="1"/>
+        <v>5.9582291666883975</v>
+      </c>
+      <c r="C73" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
+        <v>1355171695493</v>
+      </c>
+      <c r="B74" s="2">
+        <f t="shared" si="1"/>
+        <v>6.0416813889169134</v>
+      </c>
+      <c r="C74" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="4">
+        <v>1355171996212</v>
+      </c>
+      <c r="B75" s="2">
+        <f t="shared" si="1"/>
+        <v>6.1252144444733858</v>
+      </c>
+      <c r="C75" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="4">
+        <v>1355172295341</v>
+      </c>
+      <c r="B76" s="2">
+        <f t="shared" si="1"/>
+        <v>6.2083058333373629</v>
+      </c>
+      <c r="C76" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="4">
+        <v>1355172596055</v>
+      </c>
+      <c r="B77" s="2">
+        <f t="shared" si="1"/>
+        <v>6.2918375000008382</v>
+      </c>
+      <c r="C77" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="4">
+        <v>1355172896066</v>
+      </c>
+      <c r="B78" s="2">
+        <f t="shared" si="1"/>
+        <v>6.375173888867721</v>
+      </c>
+      <c r="C78" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="4">
+        <v>1355173195202</v>
+      </c>
+      <c r="B79" s="2">
+        <f t="shared" si="1"/>
+        <v>6.4582672222168185</v>
+      </c>
+      <c r="C79" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="4">
+        <v>1355173495057</v>
+      </c>
+      <c r="B80" s="2">
+        <f t="shared" si="1"/>
+        <v>6.5415602778084576</v>
+      </c>
+      <c r="C80" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="4">
+        <v>1355173795283</v>
+      </c>
+      <c r="B81" s="2">
+        <f t="shared" si="1"/>
+        <v>6.6249563888995908</v>
+      </c>
+      <c r="C81" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="4">
+        <v>1355174095046</v>
+      </c>
+      <c r="B82" s="2">
+        <f t="shared" si="1"/>
+        <v>6.7082238888833672</v>
+      </c>
+      <c r="C82" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="4">
+        <v>1355174395201</v>
+      </c>
+      <c r="B83" s="2">
+        <f t="shared" si="1"/>
+        <v>6.7916002777637914</v>
+      </c>
+      <c r="C83" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="4">
+        <v>1355174695044</v>
+      </c>
+      <c r="B84" s="2">
+        <f t="shared" si="1"/>
+        <v>6.874889999977313</v>
+      </c>
+      <c r="C84" s="3">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="4">
+        <v>1355174995043</v>
+      </c>
+      <c r="B85" s="2">
+        <f t="shared" si="1"/>
+        <v>6.9582230555824935</v>
+      </c>
+      <c r="C85" s="3">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="4">
+        <v>1355175295048</v>
+      </c>
+      <c r="B86" s="2">
+        <f t="shared" si="1"/>
+        <v>7.0415577777894214</v>
+      </c>
+      <c r="C86" s="3">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="2"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="3"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="2"/>
+      <c r="B88" s="2"/>
+      <c r="C88" s="3"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="2"/>
+      <c r="B89" s="2"/>
+      <c r="C89" s="3"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="2"/>
+      <c r="B90" s="2"/>
+      <c r="C90" s="3"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="2"/>
+      <c r="B91" s="2"/>
+      <c r="C91" s="3"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="2"/>
+      <c r="B92" s="2"/>
+      <c r="C92" s="3"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="2"/>
+      <c r="B93" s="2"/>
+      <c r="C93" s="3"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="2"/>
+      <c r="B94" s="2"/>
+      <c r="C94" s="3"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="2"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="3"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="2"/>
+      <c r="B96" s="2"/>
+      <c r="C96" s="3"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="2"/>
+      <c r="B97" s="2"/>
+      <c r="C97" s="3"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="2"/>
+      <c r="B98" s="2"/>
+      <c r="C98" s="3"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="2"/>
+      <c r="B99" s="2"/>
+      <c r="C99" s="3"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="2"/>
+      <c r="B100" s="2"/>
+      <c r="C100" s="3"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="2"/>
+      <c r="B101" s="2"/>
+      <c r="C101" s="3"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="2"/>
+      <c r="B102" s="2"/>
+      <c r="C102" s="3"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="2"/>
+      <c r="B103" s="2"/>
+      <c r="C103" s="3"/>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="2"/>
+      <c r="B104" s="2"/>
+      <c r="C104" s="3"/>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="2"/>
+      <c r="B105" s="2"/>
+      <c r="C105" s="3"/>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="2"/>
+      <c r="B106" s="2"/>
+      <c r="C106" s="3"/>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="2"/>
+      <c r="B107" s="2"/>
+      <c r="C107" s="3"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="2"/>
+      <c r="B108" s="2"/>
+      <c r="C108" s="3"/>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="2"/>
+      <c r="B109" s="2"/>
+      <c r="C109" s="3"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="2"/>
+      <c r="B110" s="2"/>
+      <c r="C110" s="3"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="2"/>
+      <c r="B111" s="2"/>
+      <c r="C111" s="3"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="2"/>
+      <c r="B112" s="2"/>
+      <c r="C112" s="3"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="2"/>
+      <c r="B113" s="2"/>
+      <c r="C113" s="3"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="2"/>
+      <c r="B114" s="2"/>
+      <c r="C114" s="3"/>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="2"/>
+      <c r="B115" s="2"/>
+      <c r="C115" s="3"/>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="2"/>
+      <c r="B116" s="2"/>
+      <c r="C116" s="3"/>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="2"/>
+      <c r="B117" s="2"/>
+      <c r="C117" s="3"/>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="2"/>
+      <c r="B118" s="2"/>
+      <c r="C118" s="3"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="2"/>
+      <c r="B119" s="2"/>
+      <c r="C119" s="3"/>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="2"/>
+      <c r="B120" s="2"/>
+      <c r="C120" s="3"/>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="2"/>
+      <c r="B121" s="2"/>
+      <c r="C121" s="3"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="2"/>
+      <c r="B122" s="2"/>
+      <c r="C122" s="3"/>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="2"/>
+      <c r="B123" s="2"/>
+      <c r="C123" s="3"/>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="2"/>
+      <c r="B124" s="2"/>
+      <c r="C124" s="3"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="2"/>
+      <c r="B125" s="2"/>
+      <c r="C125" s="3"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="2"/>
+      <c r="B126" s="2"/>
+      <c r="C126" s="3"/>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="2"/>
+      <c r="B127" s="2"/>
+      <c r="C127" s="3"/>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="2"/>
+      <c r="B128" s="2"/>
+      <c r="C128" s="3"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="2"/>
+      <c r="B129" s="2"/>
+      <c r="C129" s="3"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="2"/>
+      <c r="B130" s="2"/>
+      <c r="C130" s="3"/>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="2"/>
+      <c r="B131" s="2"/>
+      <c r="C131" s="3"/>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="2"/>
+      <c r="B132" s="2"/>
+      <c r="C132" s="3"/>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="2"/>
+      <c r="B133" s="2"/>
+      <c r="C133" s="3"/>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="2"/>
+      <c r="B134" s="2"/>
+      <c r="C134" s="3"/>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="2"/>
+      <c r="B135" s="2"/>
+      <c r="C135" s="3"/>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="2"/>
+      <c r="B136" s="2"/>
+      <c r="C136" s="3"/>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="2"/>
+      <c r="B137" s="2"/>
+      <c r="C137" s="3"/>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="2"/>
+      <c r="B138" s="2"/>
+      <c r="C138" s="3"/>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="2"/>
+      <c r="B139" s="2"/>
+      <c r="C139" s="3"/>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="2"/>
+      <c r="B140" s="2"/>
+      <c r="C140" s="3"/>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="2"/>
+      <c r="B141" s="2"/>
+      <c r="C141" s="3"/>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="2"/>
+      <c r="B142" s="2"/>
+      <c r="C142" s="3"/>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="2"/>
+      <c r="B143" s="2"/>
+      <c r="C143" s="3"/>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="2"/>
+      <c r="B144" s="2"/>
+      <c r="C144" s="3"/>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="2"/>
+      <c r="B145" s="2"/>
+      <c r="C145" s="3"/>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="2"/>
+      <c r="B146" s="2"/>
+      <c r="C146" s="3"/>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="2"/>
+      <c r="B147" s="2"/>
+      <c r="C147" s="3"/>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="2"/>
+      <c r="B148" s="2"/>
+      <c r="C148" s="3"/>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="2"/>
+      <c r="B149" s="2"/>
+      <c r="C149" s="3"/>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="2"/>
+      <c r="B150" s="2"/>
+      <c r="C150" s="3"/>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="2"/>
+      <c r="B151" s="2"/>
+      <c r="C151" s="3"/>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="2"/>
+      <c r="B152" s="2"/>
+      <c r="C152" s="3"/>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="2"/>
+      <c r="B153" s="2"/>
+      <c r="C153" s="3"/>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="2"/>
+      <c r="B154" s="2"/>
+      <c r="C154" s="3"/>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="2"/>
+      <c r="B155" s="2"/>
+      <c r="C155" s="3"/>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="2"/>
+      <c r="B156" s="2"/>
+      <c r="C156" s="3"/>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="2"/>
+      <c r="B157" s="2"/>
+      <c r="C157" s="3"/>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="2"/>
+      <c r="B158" s="2"/>
+      <c r="C158" s="3"/>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="2"/>
+      <c r="B159" s="2"/>
+      <c r="C159" s="3"/>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="2"/>
+      <c r="B160" s="2"/>
+      <c r="C160" s="3"/>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="2"/>
+      <c r="B161" s="2"/>
+      <c r="C161" s="3"/>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="2"/>
+      <c r="B162" s="2"/>
+      <c r="C162" s="3"/>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="2"/>
+      <c r="B163" s="2"/>
+      <c r="C163" s="3"/>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="2"/>
+      <c r="B164" s="2"/>
+      <c r="C164" s="3"/>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="2"/>
+      <c r="B165" s="2"/>
+      <c r="C165" s="3"/>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="2"/>
+      <c r="B166" s="2"/>
+      <c r="C166" s="3"/>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="2"/>
+      <c r="B167" s="2"/>
+      <c r="C167" s="3"/>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="2"/>
+      <c r="B168" s="2"/>
+      <c r="C168" s="3"/>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="2"/>
+      <c r="B169" s="2"/>
+      <c r="C169" s="3"/>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="2"/>
+      <c r="B170" s="2"/>
+      <c r="C170" s="3"/>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="2"/>
+      <c r="B171" s="2"/>
+      <c r="C171" s="3"/>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="2"/>
+      <c r="B172" s="2"/>
+      <c r="C172" s="3"/>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" s="2"/>
+      <c r="B173" s="2"/>
+      <c r="C173" s="3"/>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="2"/>
+      <c r="B174" s="2"/>
+      <c r="C174" s="3"/>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="2"/>
+      <c r="B175" s="2"/>
+      <c r="C175" s="3"/>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="2"/>
+      <c r="B176" s="2"/>
+      <c r="C176" s="3"/>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" s="2"/>
+      <c r="B177" s="2"/>
+      <c r="C177" s="3"/>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="2"/>
+      <c r="B178" s="2"/>
+      <c r="C178" s="3"/>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" s="2"/>
+      <c r="B179" s="2"/>
+      <c r="C179" s="3"/>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" s="2"/>
+      <c r="B180" s="2"/>
+      <c r="C180" s="3"/>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" s="2"/>
+      <c r="B181" s="2"/>
+      <c r="C181" s="3"/>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" s="2"/>
+      <c r="B182" s="2"/>
+      <c r="C182" s="3"/>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" s="2"/>
+      <c r="B183" s="2"/>
+      <c r="C183" s="3"/>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" s="2"/>
+      <c r="B184" s="2"/>
+      <c r="C184" s="3"/>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" s="2"/>
+      <c r="B185" s="2"/>
+      <c r="C185" s="3"/>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" s="2"/>
+      <c r="B186" s="2"/>
+      <c r="C186" s="3"/>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" s="2"/>
+      <c r="B187" s="2"/>
+      <c r="C187" s="3"/>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="2"/>
+      <c r="B188" s="2"/>
+      <c r="C188" s="3"/>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" s="2"/>
+      <c r="B189" s="2"/>
+      <c r="C189" s="3"/>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" s="2"/>
+      <c r="B190" s="2"/>
+      <c r="C190" s="3"/>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" s="2"/>
+      <c r="B191" s="2"/>
+      <c r="C191" s="3"/>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" s="2"/>
+      <c r="B192" s="2"/>
+      <c r="C192" s="3"/>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" s="2"/>
+      <c r="B193" s="2"/>
+      <c r="C193" s="3"/>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" s="2"/>
+      <c r="B194" s="2"/>
+      <c r="C194" s="3"/>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" s="2"/>
+      <c r="B195" s="2"/>
+      <c r="C195" s="3"/>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" s="2"/>
+      <c r="B196" s="2"/>
+      <c r="C196" s="3"/>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" s="2"/>
+      <c r="B197" s="2"/>
+      <c r="C197" s="3"/>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" s="2"/>
+      <c r="B198" s="2"/>
+      <c r="C198" s="3"/>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" s="2"/>
+      <c r="B199" s="2"/>
+      <c r="C199" s="3"/>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" s="2"/>
+      <c r="B200" s="2"/>
+      <c r="C200" s="3"/>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" s="2"/>
+      <c r="B201" s="2"/>
+      <c r="C201" s="3"/>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" s="2"/>
+      <c r="B202" s="2"/>
+      <c r="C202" s="3"/>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" s="2"/>
+      <c r="B203" s="2"/>
+      <c r="C203" s="3"/>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" s="2"/>
+      <c r="B204" s="2"/>
+      <c r="C204" s="3"/>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" s="2"/>
+      <c r="B205" s="2"/>
+      <c r="C205" s="3"/>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" s="2"/>
+      <c r="B206" s="2"/>
+      <c r="C206" s="3"/>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" s="2"/>
+      <c r="B207" s="2"/>
+      <c r="C207" s="3"/>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" s="2"/>
+      <c r="B208" s="2"/>
+      <c r="C208" s="3"/>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" s="2"/>
+      <c r="B209" s="2"/>
+      <c r="C209" s="3"/>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" s="2"/>
+      <c r="B210" s="2"/>
+      <c r="C210" s="3"/>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" s="2"/>
+      <c r="B211" s="2"/>
+      <c r="C211" s="3"/>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" s="2"/>
+      <c r="B212" s="2"/>
+      <c r="C212" s="3"/>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" s="2"/>
+      <c r="B213" s="2"/>
+      <c r="C213" s="3"/>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" s="2"/>
+      <c r="B214" s="2"/>
+      <c r="C214" s="3"/>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" s="2"/>
+      <c r="B215" s="2"/>
+      <c r="C215" s="3"/>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216" s="2"/>
+      <c r="B216" s="2"/>
+      <c r="C216" s="3"/>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217" s="2"/>
+      <c r="B217" s="2"/>
+      <c r="C217" s="3"/>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218" s="2"/>
+      <c r="B218" s="2"/>
+      <c r="C218" s="3"/>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" s="2"/>
+      <c r="B219" s="2"/>
+      <c r="C219" s="3"/>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" s="2"/>
+      <c r="B220" s="2"/>
+      <c r="C220" s="3"/>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" s="2"/>
+      <c r="B221" s="2"/>
+      <c r="C221" s="3"/>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" s="2"/>
+      <c r="B222" s="2"/>
+      <c r="C222" s="3"/>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223" s="2"/>
+      <c r="B223" s="2"/>
+      <c r="C223" s="3"/>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224" s="2"/>
+      <c r="B224" s="2"/>
+      <c r="C224" s="3"/>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225" s="2"/>
+      <c r="B225" s="2"/>
+      <c r="C225" s="3"/>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226" s="2"/>
+      <c r="B226" s="2"/>
+      <c r="C226" s="3"/>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" s="2"/>
+      <c r="B227" s="2"/>
+      <c r="C227" s="3"/>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" s="2"/>
+      <c r="B228" s="2"/>
+      <c r="C228" s="3"/>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" s="2"/>
+      <c r="B229" s="2"/>
+      <c r="C229" s="3"/>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" s="2"/>
+      <c r="B230" s="2"/>
+      <c r="C230" s="3"/>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231" s="2"/>
+      <c r="B231" s="2"/>
+      <c r="C231" s="3"/>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232" s="2"/>
+      <c r="B232" s="2"/>
+      <c r="C232" s="3"/>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233" s="2"/>
+      <c r="B233" s="2"/>
+      <c r="C233" s="3"/>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234" s="2"/>
+      <c r="B234" s="2"/>
+      <c r="C234" s="3"/>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235" s="2"/>
+      <c r="B235" s="2"/>
+      <c r="C235" s="3"/>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236" s="2"/>
+      <c r="B236" s="2"/>
+      <c r="C236" s="3"/>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237" s="2"/>
+      <c r="B237" s="2"/>
+      <c r="C237" s="3"/>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238" s="2"/>
+      <c r="B238" s="2"/>
+      <c r="C238" s="3"/>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A239" s="2"/>
+      <c r="B239" s="2"/>
+      <c r="C239" s="3"/>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A240" s="2"/>
+      <c r="B240" s="2"/>
+      <c r="C240" s="3"/>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241" s="2"/>
+      <c r="B241" s="2"/>
+      <c r="C241" s="3"/>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" s="2"/>
+      <c r="B242" s="2"/>
+      <c r="C242" s="3"/>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" s="2"/>
+      <c r="B243" s="2"/>
+      <c r="C243" s="3"/>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244" s="2"/>
+      <c r="B244" s="2"/>
+      <c r="C244" s="3"/>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245" s="2"/>
+      <c r="B245" s="2"/>
+      <c r="C245" s="3"/>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A246" s="2"/>
+      <c r="B246" s="2"/>
+      <c r="C246" s="3"/>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A247" s="2"/>
+      <c r="B247" s="2"/>
+      <c r="C247" s="3"/>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A248" s="2"/>
+      <c r="B248" s="2"/>
+      <c r="C248" s="3"/>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A249" s="2"/>
+      <c r="B249" s="2"/>
+      <c r="C249" s="3"/>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A250" s="2"/>
+      <c r="B250" s="2"/>
+      <c r="C250" s="3"/>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A251" s="2"/>
+      <c r="B251" s="2"/>
+      <c r="C251" s="3"/>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A252" s="2"/>
+      <c r="B252" s="2"/>
+      <c r="C252" s="3"/>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A253" s="2"/>
+      <c r="B253" s="2"/>
+      <c r="C253" s="3"/>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A254" s="2"/>
+      <c r="B254" s="2"/>
+      <c r="C254" s="3"/>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A255" s="2"/>
+      <c r="B255" s="2"/>
+      <c r="C255" s="3"/>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A256" s="2"/>
+      <c r="B256" s="2"/>
+      <c r="C256" s="3"/>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A257" s="2"/>
+      <c r="B257" s="2"/>
+      <c r="C257" s="3"/>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A258" s="2"/>
+      <c r="B258" s="2"/>
+      <c r="C258" s="3"/>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A259" s="2"/>
+      <c r="B259" s="2"/>
+      <c r="C259" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updating the pretty charts.
</commit_message>
<xml_diff>
--- a/data/Android Battery Charts.xlsx
+++ b/data/Android Battery Charts.xlsx
@@ -331,11 +331,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="112741184"/>
-        <c:axId val="112741760"/>
+        <c:axId val="75124672"/>
+        <c:axId val="75125248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="112741184"/>
+        <c:axId val="75124672"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -345,12 +345,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112741760"/>
+        <c:crossAx val="75125248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="112741760"/>
+        <c:axId val="75125248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -361,14 +361,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112741184"/>
+        <c:crossAx val="75124672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -497,11 +496,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="124772928"/>
-        <c:axId val="124773504"/>
+        <c:axId val="111002176"/>
+        <c:axId val="111002752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="124772928"/>
+        <c:axId val="111002176"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -511,12 +510,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124773504"/>
+        <c:crossAx val="111002752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="124773504"/>
+        <c:axId val="111002752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -527,14 +526,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124772928"/>
+        <c:crossAx val="111002176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -564,7 +562,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -670,11 +667,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="124775808"/>
-        <c:axId val="124776384"/>
+        <c:axId val="111004480"/>
+        <c:axId val="111005056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="124775808"/>
+        <c:axId val="111004480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -701,19 +698,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124776384"/>
+        <c:crossAx val="111005056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="124776384"/>
+        <c:axId val="111005056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -741,14 +737,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124775808"/>
+        <c:crossAx val="111004480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -798,34 +793,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:trendline>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-1.9900304081468864E-2"/>
-                  <c:y val="-0.66127008310443003"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:trendline>
-            <c:trendlineType val="exp"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-3.7506948098078904E-2"/>
-                  <c:y val="-0.47697411729637795"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Battery Level 4'!$B$2:$B$259</c:f>
@@ -1364,11 +1331,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="124778112"/>
-        <c:axId val="124778688"/>
+        <c:axId val="111006784"/>
+        <c:axId val="111007360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="124778112"/>
+        <c:axId val="111006784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="7"/>
@@ -1403,12 +1370,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124778688"/>
+        <c:crossAx val="111007360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="124778688"/>
+        <c:axId val="111007360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1440,7 +1407,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124778112"/>
+        <c:crossAx val="111006784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1472,7 +1439,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1588,11 +1554,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="127699200"/>
-        <c:axId val="127699776"/>
+        <c:axId val="111009088"/>
+        <c:axId val="112656384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="127699200"/>
+        <c:axId val="111009088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1619,19 +1585,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127699776"/>
+        <c:crossAx val="112656384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="127699776"/>
+        <c:axId val="112656384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1659,14 +1624,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127699200"/>
+        <c:crossAx val="111009088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1698,7 +1662,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1924,11 +1887,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="112743488"/>
-        <c:axId val="112744064"/>
+        <c:axId val="75126976"/>
+        <c:axId val="75127552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="112743488"/>
+        <c:axId val="75126976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1955,19 +1918,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112744064"/>
+        <c:crossAx val="75127552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="112744064"/>
+        <c:axId val="75127552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1995,14 +1957,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112743488"/>
+        <c:crossAx val="75126976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2034,7 +1995,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3628,11 +3588,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="112745792"/>
-        <c:axId val="115097600"/>
+        <c:axId val="105333312"/>
+        <c:axId val="105333888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="112745792"/>
+        <c:axId val="105333312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3659,19 +3619,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115097600"/>
+        <c:crossAx val="105333888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115097600"/>
+        <c:axId val="105333888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3694,14 +3653,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112745792"/>
+        <c:crossAx val="105333312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3802,11 +3760,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="115099328"/>
-        <c:axId val="115099904"/>
+        <c:axId val="105335616"/>
+        <c:axId val="105336192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115099328"/>
+        <c:axId val="105335616"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3816,12 +3774,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115099904"/>
+        <c:crossAx val="105336192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115099904"/>
+        <c:axId val="105336192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3832,7 +3790,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115099328"/>
+        <c:crossAx val="105335616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3937,11 +3895,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="115101632"/>
-        <c:axId val="115102208"/>
+        <c:axId val="105337920"/>
+        <c:axId val="105338496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115101632"/>
+        <c:axId val="105337920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3951,12 +3909,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115102208"/>
+        <c:crossAx val="105338496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115102208"/>
+        <c:axId val="105338496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3967,7 +3925,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115101632"/>
+        <c:crossAx val="105337920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5647,11 +5605,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="115103936"/>
-        <c:axId val="115104512"/>
+        <c:axId val="105340224"/>
+        <c:axId val="108961792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115103936"/>
+        <c:axId val="105340224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5661,12 +5619,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115104512"/>
+        <c:crossAx val="108961792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115104512"/>
+        <c:axId val="108961792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5677,7 +5635,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115103936"/>
+        <c:crossAx val="105340224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5758,11 +5716,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="116499008"/>
-        <c:axId val="116499584"/>
+        <c:axId val="108963520"/>
+        <c:axId val="108964096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="116499008"/>
+        <c:axId val="108963520"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -5772,12 +5730,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116499584"/>
+        <c:crossAx val="108964096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="116499584"/>
+        <c:axId val="108964096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5788,7 +5746,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116499008"/>
+        <c:crossAx val="108963520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5869,11 +5827,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="116501312"/>
-        <c:axId val="116501888"/>
+        <c:axId val="108965824"/>
+        <c:axId val="108966400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="116501312"/>
+        <c:axId val="108965824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5883,12 +5841,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116501888"/>
+        <c:crossAx val="108966400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="116501888"/>
+        <c:axId val="108966400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5899,7 +5857,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116501312"/>
+        <c:crossAx val="108965824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6012,11 +5970,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="116503616"/>
-        <c:axId val="116504192"/>
+        <c:axId val="108968128"/>
+        <c:axId val="108968704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="116503616"/>
+        <c:axId val="108968128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6026,12 +5984,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116504192"/>
+        <c:crossAx val="108968704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="116504192"/>
+        <c:axId val="108968704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6042,7 +6000,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116503616"/>
+        <c:crossAx val="108968128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -16170,7 +16128,7 @@
         <v>1355156064036</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" ref="C3:C31" si="0">B3/(1000*3600)-$C$1</f>
+        <f t="shared" ref="C3:C11" si="0">B3/(1000*3600)-$C$1</f>
         <v>0.66660666669486091</v>
       </c>
       <c r="D3">
@@ -16183,15 +16141,15 @@
         <v>0.95</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H31" si="1">IF(D3=0,F3/E3,F3/D3)</f>
+        <f t="shared" ref="H3:H11" si="1">IF(D3=0,F3/E3,F3/D3)</f>
         <v>145316654.99999997</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I31" si="2">H3/(1000*60)</f>
+        <f t="shared" ref="I3:I11" si="2">H3/(1000*60)</f>
         <v>2421.9442499999996</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J31" si="3">I3/60</f>
+        <f t="shared" ref="J3:J11" si="3">I3/60</f>
         <v>40.365737499999994</v>
       </c>
     </row>
@@ -16586,7 +16544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D259"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -17389,7 +17347,7 @@
         <v>1355169595034</v>
       </c>
       <c r="B67" s="2">
-        <f t="shared" ref="B67:B130" si="1">A67/(1000*3600)-$D$1</f>
+        <f t="shared" ref="B67:B86" si="1">A67/(1000*3600)-$D$1</f>
         <v>5.4582205555634573</v>
       </c>
       <c r="C67" s="3">

</xml_diff>